<commit_message>
Task09 presentation und Excel aktualisiert
</commit_message>
<xml_diff>
--- a/doc/task06/Scrum_v0.7.xlsx
+++ b/doc/task06/Scrum_v0.7.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajilatha.kandiah\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klembowski_r\Desktop\zeug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE07980-8885-4140-AD33-8B6F6507E782}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19368" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -496,7 +495,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,6 +685,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -694,26 +694,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -722,8 +702,170 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43593</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8B48-41C4-A237-FD0E08BA7A94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Ressources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43593</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43598</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43601</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8B48-41C4-A237-FD0E08BA7A94}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>BurndownChart!$D$1</c:f>
@@ -823,13 +965,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-32DF-4ACB-B206-BE37E6124221}"/>
+              <c16:uniqueId val="{00000001-8B48-41C4-A237-FD0E08BA7A94}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>BurndownChart!$E$1</c:f>
@@ -929,7 +1071,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-32DF-4ACB-B206-BE37E6124221}"/>
+              <c16:uniqueId val="{00000003-8B48-41C4-A237-FD0E08BA7A94}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1044,16 +1186,10 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1085,6 +1221,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1092,23 +1229,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -1167,6 +1288,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1547,6 +1669,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1578,6 +1701,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1585,7 +1709,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1602,6 +1725,561 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart Sprint 3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A020-4F5A-8CBF-4055661A0B5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Ressources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$E$17:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A020-4F5A-8CBF-4055661A0B5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A020-4F5A-8CBF-4055661A0B5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BurndownChart!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Ressources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>BurndownChart!$C$17:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43619</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43626</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BurndownChart!$E$17:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A020-4F5A-8CBF-4055661A0B5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="574879000"/>
+        <c:axId val="395058816"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="574879000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="395058816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="395058816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="574879000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -1660,568 +2338,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2818,6 +2935,44 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>6531</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F887DE1-CC1F-4A40-AD9A-1107B83CC6E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2897,23 +3052,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2949,23 +3087,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3141,20 +3262,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3162,7 +3283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3170,7 +3291,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -3178,7 +3299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -3186,7 +3307,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -3194,7 +3315,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -3202,7 +3323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -3212,38 +3333,38 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/smowdy" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/ceoy" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/raji98" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://github.com/nristicBFH" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://github.com/suttc1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B5" r:id="rId6" display="https://github.com/DerRaphe" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/smowdy"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/ceoy"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/raji98"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://github.com/nristicBFH"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://github.com/suttc1"/>
+    <hyperlink ref="B5" r:id="rId6" display="https://github.com/DerRaphe"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.86328125" customWidth="1"/>
-    <col min="2" max="2" width="24.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.86328125" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" customWidth="1"/>
-    <col min="5" max="5" width="11.86328125" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
-    <col min="7" max="7" width="10.1328125" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3269,7 +3390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -3295,7 +3416,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -3321,7 +3442,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -3347,7 +3468,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -3373,7 +3494,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -3399,7 +3520,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -3425,7 +3546,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -3451,7 +3572,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -3477,7 +3598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E11">
         <f>SUM(E2:E9)</f>
         <v>144</v>
@@ -3498,29 +3619,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="A47" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1328125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1328125" customWidth="1"/>
-    <col min="7" max="7" width="9.86328125" customWidth="1"/>
-    <col min="8" max="8" width="8.1328125" customWidth="1"/>
-    <col min="9" max="9" width="7.86328125" customWidth="1"/>
-    <col min="10" max="10" width="7.1328125" customWidth="1"/>
-    <col min="11" max="11" width="15.1328125" customWidth="1"/>
+    <col min="4" max="4" width="52.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3555,7 +3676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>2</v>
       </c>
@@ -3586,7 +3707,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2.1</v>
       </c>
@@ -3618,7 +3739,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>2.2000000000000002</v>
       </c>
@@ -3650,7 +3771,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>2.2999999999999998</v>
       </c>
@@ -3682,7 +3803,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>2.4</v>
       </c>
@@ -3714,7 +3835,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>2.5</v>
       </c>
@@ -3746,7 +3867,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>2.6</v>
       </c>
@@ -3778,7 +3899,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>2.7</v>
       </c>
@@ -3810,7 +3931,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>2.8</v>
       </c>
@@ -3842,7 +3963,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>2.9</v>
       </c>
@@ -3874,7 +3995,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
         <v>2.1</v>
       </c>
@@ -3906,7 +4027,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
         <v>2.11</v>
       </c>
@@ -3938,13 +4059,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" s="15"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>3</v>
       </c>
@@ -3975,7 +4096,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>3.1</v>
       </c>
@@ -4007,7 +4128,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>3.2</v>
       </c>
@@ -4039,7 +4160,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>3.3</v>
       </c>
@@ -4071,7 +4192,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>3.4</v>
       </c>
@@ -4103,7 +4224,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>3.5</v>
       </c>
@@ -4135,7 +4256,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>3.6</v>
       </c>
@@ -4167,7 +4288,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>3.7</v>
       </c>
@@ -4199,13 +4320,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K25" s="15"/>
     </row>
-    <row r="26" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>4</v>
       </c>
@@ -4234,7 +4355,7 @@
       </c>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>4.0999999999999996</v>
       </c>
@@ -4266,7 +4387,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>4.2</v>
       </c>
@@ -4298,20 +4419,20 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
       <c r="K29" s="15"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K30" s="15"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K31" s="15"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
         <v>5</v>
       </c>
@@ -4340,7 +4461,7 @@
       </c>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>5.0999999999999996</v>
       </c>
@@ -4372,7 +4493,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>5.2</v>
       </c>
@@ -4404,7 +4525,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>5.3</v>
       </c>
@@ -4436,7 +4557,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>5.4</v>
       </c>
@@ -4468,7 +4589,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>5.5</v>
       </c>
@@ -4500,7 +4621,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>5.6</v>
       </c>
@@ -4532,7 +4653,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>5.7</v>
       </c>
@@ -4564,16 +4685,16 @@
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
         <v>6</v>
       </c>
@@ -4604,7 +4725,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>6.1</v>
       </c>
@@ -4636,7 +4757,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>6.2</v>
       </c>
@@ -4668,7 +4789,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>6.3</v>
       </c>
@@ -4700,7 +4821,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <v>6.4</v>
       </c>
@@ -4732,7 +4853,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>6.5</v>
       </c>
@@ -4764,7 +4885,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <v>6.6</v>
       </c>
@@ -4796,10 +4917,10 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
         <v>7</v>
       </c>
@@ -4828,7 +4949,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>7.1</v>
       </c>
@@ -4860,7 +4981,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <v>7.2</v>
       </c>
@@ -4892,7 +5013,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>7.3</v>
       </c>
@@ -4924,7 +5045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>7.4</v>
       </c>
@@ -4956,7 +5077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>7.5</v>
       </c>
@@ -4988,7 +5109,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>7.6</v>
       </c>
@@ -5020,7 +5141,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <v>7.7</v>
       </c>
@@ -5052,13 +5173,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="14">
         <v>1</v>
       </c>
@@ -5087,7 +5208,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>1.1000000000000001</v>
       </c>
@@ -5119,7 +5240,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>1.2</v>
       </c>
@@ -5151,7 +5272,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>1.3</v>
       </c>
@@ -5183,7 +5304,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>1.4</v>
       </c>
@@ -5215,19 +5336,19 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="14">
         <v>8</v>
       </c>
@@ -5248,12 +5369,14 @@
         <f>SUM(I71:I77)</f>
         <v>20</v>
       </c>
-      <c r="J70" s="14"/>
+      <c r="J70" s="14">
+        <v>20</v>
+      </c>
       <c r="K70" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>8.1</v>
       </c>
@@ -5275,11 +5398,14 @@
       <c r="I71">
         <v>4</v>
       </c>
+      <c r="J71">
+        <v>4</v>
+      </c>
       <c r="K71" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>8.1999999999999993</v>
       </c>
@@ -5301,11 +5427,14 @@
       <c r="I72">
         <v>4</v>
       </c>
+      <c r="J72">
+        <v>4</v>
+      </c>
       <c r="K72" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>8.3000000000000007</v>
       </c>
@@ -5327,11 +5456,14 @@
       <c r="I73">
         <v>2</v>
       </c>
+      <c r="J73">
+        <v>2</v>
+      </c>
       <c r="K73" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>8.4</v>
       </c>
@@ -5353,11 +5485,14 @@
       <c r="I74">
         <v>4</v>
       </c>
+      <c r="J74">
+        <v>4</v>
+      </c>
       <c r="K74" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>8.5</v>
       </c>
@@ -5379,11 +5514,14 @@
       <c r="I75">
         <v>4</v>
       </c>
+      <c r="J75">
+        <v>4</v>
+      </c>
       <c r="K75" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
         <v>80</v>
       </c>
@@ -5399,11 +5537,14 @@
       <c r="I76">
         <v>2</v>
       </c>
+      <c r="J76">
+        <v>2</v>
+      </c>
       <c r="K76" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K77" s="8"/>
     </row>
   </sheetData>
@@ -5413,22 +5554,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.59765625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="27.86328125" customWidth="1"/>
-    <col min="6" max="6" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -5448,7 +5589,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5469,7 +5610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5490,7 +5631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5511,7 +5652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5532,7 +5673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5553,7 +5694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5574,7 +5715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5595,7 +5736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="17">
         <v>2</v>
       </c>
@@ -5615,7 +5756,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -5635,7 +5776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -5655,7 +5796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -5675,7 +5816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -5695,7 +5836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -5715,7 +5856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -5735,7 +5876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -5753,6 +5894,106 @@
       </c>
       <c r="F16">
         <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="18">
+        <v>43618</v>
+      </c>
+      <c r="D17" s="17">
+        <v>20</v>
+      </c>
+      <c r="E17" s="17">
+        <v>15</v>
+      </c>
+      <c r="F17" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>3</v>
+      </c>
+      <c r="B18" s="19">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5">
+        <v>43619</v>
+      </c>
+      <c r="D18" s="19">
+        <v>15</v>
+      </c>
+      <c r="E18" s="19">
+        <v>11</v>
+      </c>
+      <c r="F18" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>3</v>
+      </c>
+      <c r="B19" s="19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5">
+        <v>43625</v>
+      </c>
+      <c r="D19" s="19">
+        <v>11</v>
+      </c>
+      <c r="E19" s="19">
+        <v>8</v>
+      </c>
+      <c r="F19" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>3</v>
+      </c>
+      <c r="B20" s="19">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5">
+        <v>43626</v>
+      </c>
+      <c r="D20" s="19">
+        <v>8</v>
+      </c>
+      <c r="E20" s="19">
+        <v>4</v>
+      </c>
+      <c r="F20" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>3</v>
+      </c>
+      <c r="B21" s="19">
+        <v>3</v>
+      </c>
+      <c r="C21" s="5">
+        <v>43627</v>
+      </c>
+      <c r="D21" s="19">
+        <v>4</v>
+      </c>
+      <c r="E21" s="19">
+        <v>0</v>
+      </c>
+      <c r="F21" s="19">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>